<commit_message>
Added more general product category for each product
Products splitted in 11 general product category for each product:
DECORATION, OTHERS, OFFICE, BAG, HOUSEHOLD, PARTY&HOLLYDAY, JEWELRY&BEAUTY, FURNITURE, TOYS, LIGHTS, GARDEN.
</commit_message>
<xml_diff>
--- a/ClusteredProducts_manual_revised.xlsx
+++ b/ClusteredProducts_manual_revised.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_FACULTATE\DATA_SCIENCE_PRJ\GIT\DSIP-PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BF046F-F74B-4840-8F30-20898DA1BFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19B7E30-EFDB-460E-9E4D-856337C819E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11691" uniqueCount="4317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11691" uniqueCount="4316">
   <si>
     <t>Description</t>
   </si>
@@ -12974,9 +12974,6 @@
   </si>
   <si>
     <t>TOYS</t>
-  </si>
-  <si>
-    <t>LIGHT</t>
   </si>
   <si>
     <t>JEWELRY&amp;BEAUTY</t>
@@ -13356,7 +13353,7 @@
   <dimension ref="A1:D3897"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13403,7 +13400,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -15125,7 +15122,7 @@
         <v>5</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -15139,7 +15136,7 @@
         <v>5</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -15195,7 +15192,7 @@
         <v>5</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -15363,7 +15360,7 @@
         <v>214</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -15377,7 +15374,7 @@
         <v>214</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -16119,7 +16116,7 @@
         <v>286</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -16357,7 +16354,7 @@
         <v>214</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -16987,7 +16984,7 @@
         <v>365</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -17001,7 +16998,7 @@
         <v>365</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -17715,7 +17712,7 @@
         <v>5</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
@@ -17967,7 +17964,7 @@
         <v>450</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -20179,7 +20176,7 @@
         <v>4270</v>
       </c>
       <c r="D487" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.25">
@@ -20193,7 +20190,7 @@
         <v>643</v>
       </c>
       <c r="D488" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.25">
@@ -20207,7 +20204,7 @@
         <v>4306</v>
       </c>
       <c r="D489" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.25">
@@ -20221,7 +20218,7 @@
         <v>643</v>
       </c>
       <c r="D490" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.25">
@@ -20235,7 +20232,7 @@
         <v>643</v>
       </c>
       <c r="D491" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.25">
@@ -20249,7 +20246,7 @@
         <v>4270</v>
       </c>
       <c r="D492" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.25">
@@ -20263,7 +20260,7 @@
         <v>4270</v>
       </c>
       <c r="D493" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.25">
@@ -20277,7 +20274,7 @@
         <v>4270</v>
       </c>
       <c r="D494" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.25">
@@ -21159,7 +21156,7 @@
         <v>5</v>
       </c>
       <c r="D557" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="558" spans="1:4" x14ac:dyDescent="0.25">
@@ -24785,7 +24782,7 @@
         <v>4306</v>
       </c>
       <c r="D816" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="817" spans="1:4" x14ac:dyDescent="0.25">
@@ -25583,7 +25580,7 @@
         <v>5</v>
       </c>
       <c r="D873" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="874" spans="1:4" x14ac:dyDescent="0.25">
@@ -28551,7 +28548,7 @@
         <v>5</v>
       </c>
       <c r="D1085" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="1086" spans="1:4" x14ac:dyDescent="0.25">
@@ -29349,7 +29346,7 @@
         <v>4278</v>
       </c>
       <c r="D1142" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1143" spans="1:4" x14ac:dyDescent="0.25">
@@ -29363,7 +29360,7 @@
         <v>4294</v>
       </c>
       <c r="D1143" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1144" spans="1:4" x14ac:dyDescent="0.25">
@@ -29377,7 +29374,7 @@
         <v>4294</v>
       </c>
       <c r="D1144" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1145" spans="1:4" x14ac:dyDescent="0.25">
@@ -29699,7 +29696,7 @@
         <v>1393</v>
       </c>
       <c r="D1167" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1168" spans="1:4" x14ac:dyDescent="0.25">
@@ -29713,7 +29710,7 @@
         <v>1393</v>
       </c>
       <c r="D1168" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1169" spans="1:4" x14ac:dyDescent="0.25">
@@ -29727,7 +29724,7 @@
         <v>1393</v>
       </c>
       <c r="D1169" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1170" spans="1:4" x14ac:dyDescent="0.25">
@@ -29741,7 +29738,7 @@
         <v>1393</v>
       </c>
       <c r="D1170" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1171" spans="1:4" x14ac:dyDescent="0.25">
@@ -29769,7 +29766,7 @@
         <v>4306</v>
       </c>
       <c r="D1172" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1173" spans="1:4" x14ac:dyDescent="0.25">
@@ -29783,7 +29780,7 @@
         <v>4270</v>
       </c>
       <c r="D1173" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1174" spans="1:4" x14ac:dyDescent="0.25">
@@ -29797,7 +29794,7 @@
         <v>4270</v>
       </c>
       <c r="D1174" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1175" spans="1:4" x14ac:dyDescent="0.25">
@@ -29811,7 +29808,7 @@
         <v>4294</v>
       </c>
       <c r="D1175" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1176" spans="1:4" x14ac:dyDescent="0.25">
@@ -29825,7 +29822,7 @@
         <v>4294</v>
       </c>
       <c r="D1176" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1177" spans="1:4" x14ac:dyDescent="0.25">
@@ -29839,7 +29836,7 @@
         <v>4283</v>
       </c>
       <c r="D1177" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1178" spans="1:4" x14ac:dyDescent="0.25">
@@ -29853,7 +29850,7 @@
         <v>4290</v>
       </c>
       <c r="D1178" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1179" spans="1:4" x14ac:dyDescent="0.25">
@@ -31043,7 +31040,7 @@
         <v>4306</v>
       </c>
       <c r="D1263" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1264" spans="1:4" x14ac:dyDescent="0.25">
@@ -33073,7 +33070,7 @@
         <v>1651</v>
       </c>
       <c r="D1408" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1409" spans="1:4" x14ac:dyDescent="0.25">
@@ -33143,7 +33140,7 @@
         <v>214</v>
       </c>
       <c r="D1413" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="1414" spans="1:4" x14ac:dyDescent="0.25">
@@ -33423,7 +33420,7 @@
         <v>4294</v>
       </c>
       <c r="D1433" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1434" spans="1:4" x14ac:dyDescent="0.25">
@@ -33437,7 +33434,7 @@
         <v>4270</v>
       </c>
       <c r="D1434" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1435" spans="1:4" x14ac:dyDescent="0.25">
@@ -33451,7 +33448,7 @@
         <v>1682</v>
       </c>
       <c r="D1435" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1436" spans="1:4" x14ac:dyDescent="0.25">
@@ -33465,7 +33462,7 @@
         <v>4294</v>
       </c>
       <c r="D1436" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1437" spans="1:4" x14ac:dyDescent="0.25">
@@ -33969,7 +33966,7 @@
         <v>4306</v>
       </c>
       <c r="D1472" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1473" spans="1:4" x14ac:dyDescent="0.25">
@@ -34445,7 +34442,7 @@
         <v>4306</v>
       </c>
       <c r="D1506" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1507" spans="1:4" x14ac:dyDescent="0.25">
@@ -34459,7 +34456,7 @@
         <v>4278</v>
       </c>
       <c r="D1507" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1508" spans="1:4" x14ac:dyDescent="0.25">
@@ -34529,7 +34526,7 @@
         <v>4306</v>
       </c>
       <c r="D1512" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1513" spans="1:4" x14ac:dyDescent="0.25">
@@ -34543,7 +34540,7 @@
         <v>4306</v>
       </c>
       <c r="D1513" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1514" spans="1:4" x14ac:dyDescent="0.25">
@@ -35019,7 +35016,7 @@
         <v>4306</v>
       </c>
       <c r="D1547" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1548" spans="1:4" x14ac:dyDescent="0.25">
@@ -35481,7 +35478,7 @@
         <v>214</v>
       </c>
       <c r="D1580" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="1581" spans="1:4" x14ac:dyDescent="0.25">
@@ -35509,7 +35506,7 @@
         <v>1651</v>
       </c>
       <c r="D1582" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1583" spans="1:4" x14ac:dyDescent="0.25">
@@ -35663,7 +35660,7 @@
         <v>1849</v>
       </c>
       <c r="D1593" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1594" spans="1:4" x14ac:dyDescent="0.25">
@@ -36321,7 +36318,7 @@
         <v>1651</v>
       </c>
       <c r="D1640" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1641" spans="1:4" x14ac:dyDescent="0.25">
@@ -36335,7 +36332,7 @@
         <v>1651</v>
       </c>
       <c r="D1641" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1642" spans="1:4" x14ac:dyDescent="0.25">
@@ -36797,7 +36794,7 @@
         <v>4270</v>
       </c>
       <c r="D1674" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1675" spans="1:4" x14ac:dyDescent="0.25">
@@ -36811,7 +36808,7 @@
         <v>4270</v>
       </c>
       <c r="D1675" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1676" spans="1:4" x14ac:dyDescent="0.25">
@@ -38071,7 +38068,7 @@
         <v>286</v>
       </c>
       <c r="D1765" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="1766" spans="1:4" x14ac:dyDescent="0.25">
@@ -38505,7 +38502,7 @@
         <v>4294</v>
       </c>
       <c r="D1796" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1797" spans="1:4" x14ac:dyDescent="0.25">
@@ -38519,7 +38516,7 @@
         <v>2062</v>
       </c>
       <c r="D1797" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1798" spans="1:4" x14ac:dyDescent="0.25">
@@ -39191,7 +39188,7 @@
         <v>214</v>
       </c>
       <c r="D1845" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="1846" spans="1:4" x14ac:dyDescent="0.25">
@@ -39653,7 +39650,7 @@
         <v>4278</v>
       </c>
       <c r="D1878" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1879" spans="1:4" x14ac:dyDescent="0.25">
@@ -39709,7 +39706,7 @@
         <v>4270</v>
       </c>
       <c r="D1882" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1883" spans="1:4" x14ac:dyDescent="0.25">
@@ -39723,7 +39720,7 @@
         <v>4270</v>
       </c>
       <c r="D1883" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1884" spans="1:4" x14ac:dyDescent="0.25">
@@ -40423,7 +40420,7 @@
         <v>2208</v>
       </c>
       <c r="D1933" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1934" spans="1:4" x14ac:dyDescent="0.25">
@@ -40437,7 +40434,7 @@
         <v>4270</v>
       </c>
       <c r="D1934" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1935" spans="1:4" x14ac:dyDescent="0.25">
@@ -40493,7 +40490,7 @@
         <v>2215</v>
       </c>
       <c r="D1938" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1939" spans="1:4" x14ac:dyDescent="0.25">
@@ -41025,7 +41022,7 @@
         <v>4291</v>
       </c>
       <c r="D1976" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="1977" spans="1:4" x14ac:dyDescent="0.25">
@@ -42089,7 +42086,7 @@
         <v>1393</v>
       </c>
       <c r="D2052" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2053" spans="1:4" x14ac:dyDescent="0.25">
@@ -42649,7 +42646,7 @@
         <v>4290</v>
       </c>
       <c r="D2092" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2093" spans="1:4" x14ac:dyDescent="0.25">
@@ -42663,7 +42660,7 @@
         <v>4283</v>
       </c>
       <c r="D2093" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2094" spans="1:4" x14ac:dyDescent="0.25">
@@ -42705,7 +42702,7 @@
         <v>4283</v>
       </c>
       <c r="D2096" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2097" spans="1:4" x14ac:dyDescent="0.25">
@@ -43195,7 +43192,7 @@
         <v>4270</v>
       </c>
       <c r="D2131" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2132" spans="1:4" x14ac:dyDescent="0.25">
@@ -43209,7 +43206,7 @@
         <v>4270</v>
       </c>
       <c r="D2132" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2133" spans="1:4" x14ac:dyDescent="0.25">
@@ -43223,7 +43220,7 @@
         <v>4270</v>
       </c>
       <c r="D2133" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2134" spans="1:4" x14ac:dyDescent="0.25">
@@ -43237,7 +43234,7 @@
         <v>4270</v>
       </c>
       <c r="D2134" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2135" spans="1:4" x14ac:dyDescent="0.25">
@@ -43251,7 +43248,7 @@
         <v>4270</v>
       </c>
       <c r="D2135" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2136" spans="1:4" x14ac:dyDescent="0.25">
@@ -43377,7 +43374,7 @@
         <v>4270</v>
       </c>
       <c r="D2144" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2145" spans="1:4" x14ac:dyDescent="0.25">
@@ -43503,7 +43500,7 @@
         <v>2442</v>
       </c>
       <c r="D2153" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2154" spans="1:4" x14ac:dyDescent="0.25">
@@ -43531,7 +43528,7 @@
         <v>4294</v>
       </c>
       <c r="D2155" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2156" spans="1:4" x14ac:dyDescent="0.25">
@@ -43545,7 +43542,7 @@
         <v>4294</v>
       </c>
       <c r="D2156" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2157" spans="1:4" x14ac:dyDescent="0.25">
@@ -43559,7 +43556,7 @@
         <v>4294</v>
       </c>
       <c r="D2157" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2158" spans="1:4" x14ac:dyDescent="0.25">
@@ -43853,7 +43850,7 @@
         <v>4306</v>
       </c>
       <c r="D2178" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2179" spans="1:4" x14ac:dyDescent="0.25">
@@ -44525,7 +44522,7 @@
         <v>1849</v>
       </c>
       <c r="D2226" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2227" spans="1:4" x14ac:dyDescent="0.25">
@@ -44539,7 +44536,7 @@
         <v>1849</v>
       </c>
       <c r="D2227" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2228" spans="1:4" x14ac:dyDescent="0.25">
@@ -44679,7 +44676,7 @@
         <v>4283</v>
       </c>
       <c r="D2237" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2238" spans="1:4" x14ac:dyDescent="0.25">
@@ -44875,7 +44872,7 @@
         <v>4306</v>
       </c>
       <c r="D2251" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2252" spans="1:4" x14ac:dyDescent="0.25">
@@ -44889,7 +44886,7 @@
         <v>4294</v>
       </c>
       <c r="D2252" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2253" spans="1:4" x14ac:dyDescent="0.25">
@@ -44903,7 +44900,7 @@
         <v>4270</v>
       </c>
       <c r="D2253" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2254" spans="1:4" x14ac:dyDescent="0.25">
@@ -44917,7 +44914,7 @@
         <v>4270</v>
       </c>
       <c r="D2254" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2255" spans="1:4" x14ac:dyDescent="0.25">
@@ -45043,7 +45040,7 @@
         <v>2557</v>
       </c>
       <c r="D2263" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2264" spans="1:4" x14ac:dyDescent="0.25">
@@ -45099,7 +45096,7 @@
         <v>4270</v>
       </c>
       <c r="D2267" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2268" spans="1:4" x14ac:dyDescent="0.25">
@@ -45113,7 +45110,7 @@
         <v>4294</v>
       </c>
       <c r="D2268" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2269" spans="1:4" x14ac:dyDescent="0.25">
@@ -45127,7 +45124,7 @@
         <v>2062</v>
       </c>
       <c r="D2269" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2270" spans="1:4" x14ac:dyDescent="0.25">
@@ -45155,7 +45152,7 @@
         <v>4294</v>
       </c>
       <c r="D2271" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2272" spans="1:4" x14ac:dyDescent="0.25">
@@ -45169,7 +45166,7 @@
         <v>4294</v>
       </c>
       <c r="D2272" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2273" spans="1:4" x14ac:dyDescent="0.25">
@@ -45617,7 +45614,7 @@
         <v>2600</v>
       </c>
       <c r="D2304" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2305" spans="1:4" x14ac:dyDescent="0.25">
@@ -45799,7 +45796,7 @@
         <v>4306</v>
       </c>
       <c r="D2317" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2318" spans="1:4" x14ac:dyDescent="0.25">
@@ -45827,7 +45824,7 @@
         <v>4290</v>
       </c>
       <c r="D2319" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2320" spans="1:4" x14ac:dyDescent="0.25">
@@ -45841,7 +45838,7 @@
         <v>4283</v>
       </c>
       <c r="D2320" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2321" spans="1:4" x14ac:dyDescent="0.25">
@@ -46415,7 +46412,7 @@
         <v>4283</v>
       </c>
       <c r="D2361" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2362" spans="1:4" x14ac:dyDescent="0.25">
@@ -46429,7 +46426,7 @@
         <v>4270</v>
       </c>
       <c r="D2362" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2363" spans="1:4" x14ac:dyDescent="0.25">
@@ -46443,7 +46440,7 @@
         <v>4283</v>
       </c>
       <c r="D2363" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2364" spans="1:4" x14ac:dyDescent="0.25">
@@ -46457,7 +46454,7 @@
         <v>4270</v>
       </c>
       <c r="D2364" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2365" spans="1:4" x14ac:dyDescent="0.25">
@@ -46471,7 +46468,7 @@
         <v>4294</v>
       </c>
       <c r="D2365" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2366" spans="1:4" x14ac:dyDescent="0.25">
@@ -46485,7 +46482,7 @@
         <v>4294</v>
       </c>
       <c r="D2366" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2367" spans="1:4" x14ac:dyDescent="0.25">
@@ -46499,7 +46496,7 @@
         <v>4294</v>
       </c>
       <c r="D2367" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2368" spans="1:4" x14ac:dyDescent="0.25">
@@ -46513,7 +46510,7 @@
         <v>2600</v>
       </c>
       <c r="D2368" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2369" spans="1:4" x14ac:dyDescent="0.25">
@@ -46527,7 +46524,7 @@
         <v>4294</v>
       </c>
       <c r="D2369" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2370" spans="1:4" x14ac:dyDescent="0.25">
@@ -46737,7 +46734,7 @@
         <v>2215</v>
       </c>
       <c r="D2384" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2385" spans="1:4" x14ac:dyDescent="0.25">
@@ -46807,7 +46804,7 @@
         <v>1651</v>
       </c>
       <c r="D2389" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2390" spans="1:4" x14ac:dyDescent="0.25">
@@ -46905,7 +46902,7 @@
         <v>4290</v>
       </c>
       <c r="D2396" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2397" spans="1:4" x14ac:dyDescent="0.25">
@@ -46919,7 +46916,7 @@
         <v>4290</v>
       </c>
       <c r="D2397" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2398" spans="1:4" x14ac:dyDescent="0.25">
@@ -46933,7 +46930,7 @@
         <v>4270</v>
       </c>
       <c r="D2398" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2399" spans="1:4" x14ac:dyDescent="0.25">
@@ -46947,7 +46944,7 @@
         <v>4270</v>
       </c>
       <c r="D2399" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2400" spans="1:4" x14ac:dyDescent="0.25">
@@ -46961,7 +46958,7 @@
         <v>4270</v>
       </c>
       <c r="D2400" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2401" spans="1:4" x14ac:dyDescent="0.25">
@@ -46975,7 +46972,7 @@
         <v>4270</v>
       </c>
       <c r="D2401" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2402" spans="1:4" x14ac:dyDescent="0.25">
@@ -47213,7 +47210,7 @@
         <v>4283</v>
       </c>
       <c r="D2418" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2419" spans="1:4" x14ac:dyDescent="0.25">
@@ -47227,7 +47224,7 @@
         <v>2719</v>
       </c>
       <c r="D2419" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2420" spans="1:4" x14ac:dyDescent="0.25">
@@ -47339,7 +47336,7 @@
         <v>4283</v>
       </c>
       <c r="D2427" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2428" spans="1:4" x14ac:dyDescent="0.25">
@@ -47717,7 +47714,7 @@
         <v>214</v>
       </c>
       <c r="D2454" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="2455" spans="1:4" x14ac:dyDescent="0.25">
@@ -47731,7 +47728,7 @@
         <v>214</v>
       </c>
       <c r="D2455" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="2456" spans="1:4" x14ac:dyDescent="0.25">
@@ -47969,7 +47966,7 @@
         <v>214</v>
       </c>
       <c r="D2472" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="2473" spans="1:4" x14ac:dyDescent="0.25">
@@ -48389,7 +48386,7 @@
         <v>4270</v>
       </c>
       <c r="D2502" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2503" spans="1:4" x14ac:dyDescent="0.25">
@@ -48403,7 +48400,7 @@
         <v>4270</v>
       </c>
       <c r="D2503" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2504" spans="1:4" x14ac:dyDescent="0.25">
@@ -48417,7 +48414,7 @@
         <v>4270</v>
       </c>
       <c r="D2504" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2505" spans="1:4" x14ac:dyDescent="0.25">
@@ -48445,7 +48442,7 @@
         <v>4270</v>
       </c>
       <c r="D2506" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2507" spans="1:4" x14ac:dyDescent="0.25">
@@ -48459,7 +48456,7 @@
         <v>4270</v>
       </c>
       <c r="D2507" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2508" spans="1:4" x14ac:dyDescent="0.25">
@@ -48473,7 +48470,7 @@
         <v>4294</v>
       </c>
       <c r="D2508" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2509" spans="1:4" x14ac:dyDescent="0.25">
@@ -48571,7 +48568,7 @@
         <v>214</v>
       </c>
       <c r="D2515" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="2516" spans="1:4" x14ac:dyDescent="0.25">
@@ -49033,7 +49030,7 @@
         <v>4270</v>
       </c>
       <c r="D2548" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2549" spans="1:4" x14ac:dyDescent="0.25">
@@ -49215,7 +49212,7 @@
         <v>1651</v>
       </c>
       <c r="D2561" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2562" spans="1:4" x14ac:dyDescent="0.25">
@@ -49229,7 +49226,7 @@
         <v>1651</v>
       </c>
       <c r="D2562" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2563" spans="1:4" x14ac:dyDescent="0.25">
@@ -49243,7 +49240,7 @@
         <v>1651</v>
       </c>
       <c r="D2563" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2564" spans="1:4" x14ac:dyDescent="0.25">
@@ -49635,7 +49632,7 @@
         <v>214</v>
       </c>
       <c r="D2591" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="2592" spans="1:4" x14ac:dyDescent="0.25">
@@ -49817,7 +49814,7 @@
         <v>1651</v>
       </c>
       <c r="D2604" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2605" spans="1:4" x14ac:dyDescent="0.25">
@@ -49971,7 +49968,7 @@
         <v>4283</v>
       </c>
       <c r="D2615" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2616" spans="1:4" x14ac:dyDescent="0.25">
@@ -49985,7 +49982,7 @@
         <v>4283</v>
       </c>
       <c r="D2616" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2617" spans="1:4" x14ac:dyDescent="0.25">
@@ -50125,7 +50122,7 @@
         <v>4270</v>
       </c>
       <c r="D2626" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2627" spans="1:4" x14ac:dyDescent="0.25">
@@ -50279,7 +50276,7 @@
         <v>4270</v>
       </c>
       <c r="D2637" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2638" spans="1:4" x14ac:dyDescent="0.25">
@@ -50293,7 +50290,7 @@
         <v>4270</v>
       </c>
       <c r="D2638" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2639" spans="1:4" x14ac:dyDescent="0.25">
@@ -50307,7 +50304,7 @@
         <v>4270</v>
       </c>
       <c r="D2639" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2640" spans="1:4" x14ac:dyDescent="0.25">
@@ -50321,7 +50318,7 @@
         <v>4294</v>
       </c>
       <c r="D2640" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2641" spans="1:4" x14ac:dyDescent="0.25">
@@ -50335,7 +50332,7 @@
         <v>4294</v>
       </c>
       <c r="D2641" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2642" spans="1:4" x14ac:dyDescent="0.25">
@@ -50349,7 +50346,7 @@
         <v>4294</v>
       </c>
       <c r="D2642" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2643" spans="1:4" x14ac:dyDescent="0.25">
@@ -50769,7 +50766,7 @@
         <v>2981</v>
       </c>
       <c r="D2672" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="2673" spans="1:4" x14ac:dyDescent="0.25">
@@ -50853,7 +50850,7 @@
         <v>4270</v>
       </c>
       <c r="D2678" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2679" spans="1:4" x14ac:dyDescent="0.25">
@@ -51049,7 +51046,7 @@
         <v>2557</v>
       </c>
       <c r="D2692" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2693" spans="1:4" x14ac:dyDescent="0.25">
@@ -51119,7 +51116,7 @@
         <v>2062</v>
       </c>
       <c r="D2697" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2698" spans="1:4" x14ac:dyDescent="0.25">
@@ -51133,7 +51130,7 @@
         <v>4270</v>
       </c>
       <c r="D2698" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2699" spans="1:4" x14ac:dyDescent="0.25">
@@ -51147,7 +51144,7 @@
         <v>4270</v>
       </c>
       <c r="D2699" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2700" spans="1:4" x14ac:dyDescent="0.25">
@@ -51161,7 +51158,7 @@
         <v>4270</v>
       </c>
       <c r="D2700" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2701" spans="1:4" x14ac:dyDescent="0.25">
@@ -51175,7 +51172,7 @@
         <v>4270</v>
       </c>
       <c r="D2701" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2702" spans="1:4" x14ac:dyDescent="0.25">
@@ -51287,7 +51284,7 @@
         <v>3022</v>
       </c>
       <c r="D2709" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2710" spans="1:4" x14ac:dyDescent="0.25">
@@ -51301,7 +51298,7 @@
         <v>4283</v>
       </c>
       <c r="D2710" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2711" spans="1:4" x14ac:dyDescent="0.25">
@@ -51315,7 +51312,7 @@
         <v>4283</v>
       </c>
       <c r="D2711" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2712" spans="1:4" x14ac:dyDescent="0.25">
@@ -51329,7 +51326,7 @@
         <v>4283</v>
       </c>
       <c r="D2712" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2713" spans="1:4" x14ac:dyDescent="0.25">
@@ -51343,7 +51340,7 @@
         <v>450</v>
       </c>
       <c r="D2713" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2714" spans="1:4" x14ac:dyDescent="0.25">
@@ -51371,7 +51368,7 @@
         <v>4294</v>
       </c>
       <c r="D2715" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2716" spans="1:4" x14ac:dyDescent="0.25">
@@ -51385,7 +51382,7 @@
         <v>2981</v>
       </c>
       <c r="D2716" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="2717" spans="1:4" x14ac:dyDescent="0.25">
@@ -51441,7 +51438,7 @@
         <v>4294</v>
       </c>
       <c r="D2720" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2721" spans="1:4" x14ac:dyDescent="0.25">
@@ -51455,7 +51452,7 @@
         <v>1682</v>
       </c>
       <c r="D2721" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2722" spans="1:4" x14ac:dyDescent="0.25">
@@ -51469,7 +51466,7 @@
         <v>1682</v>
       </c>
       <c r="D2722" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2723" spans="1:4" x14ac:dyDescent="0.25">
@@ -51483,7 +51480,7 @@
         <v>4283</v>
       </c>
       <c r="D2723" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2724" spans="1:4" x14ac:dyDescent="0.25">
@@ -51497,7 +51494,7 @@
         <v>4283</v>
       </c>
       <c r="D2724" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2725" spans="1:4" x14ac:dyDescent="0.25">
@@ -51511,7 +51508,7 @@
         <v>4283</v>
       </c>
       <c r="D2725" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2726" spans="1:4" x14ac:dyDescent="0.25">
@@ -52015,7 +52012,7 @@
         <v>4306</v>
       </c>
       <c r="D2761" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2762" spans="1:4" x14ac:dyDescent="0.25">
@@ -52029,7 +52026,7 @@
         <v>4283</v>
       </c>
       <c r="D2762" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2763" spans="1:4" x14ac:dyDescent="0.25">
@@ -52043,7 +52040,7 @@
         <v>4270</v>
       </c>
       <c r="D2763" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2764" spans="1:4" x14ac:dyDescent="0.25">
@@ -52071,7 +52068,7 @@
         <v>4294</v>
       </c>
       <c r="D2765" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2766" spans="1:4" x14ac:dyDescent="0.25">
@@ -52085,7 +52082,7 @@
         <v>4294</v>
       </c>
       <c r="D2766" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2767" spans="1:4" x14ac:dyDescent="0.25">
@@ -52099,7 +52096,7 @@
         <v>4270</v>
       </c>
       <c r="D2767" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2768" spans="1:4" x14ac:dyDescent="0.25">
@@ -52113,7 +52110,7 @@
         <v>4294</v>
       </c>
       <c r="D2768" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2769" spans="1:4" x14ac:dyDescent="0.25">
@@ -52127,7 +52124,7 @@
         <v>4294</v>
       </c>
       <c r="D2769" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2770" spans="1:4" x14ac:dyDescent="0.25">
@@ -52141,7 +52138,7 @@
         <v>4294</v>
       </c>
       <c r="D2770" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2771" spans="1:4" x14ac:dyDescent="0.25">
@@ -52155,7 +52152,7 @@
         <v>4294</v>
       </c>
       <c r="D2771" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2772" spans="1:4" x14ac:dyDescent="0.25">
@@ -52169,7 +52166,7 @@
         <v>4294</v>
       </c>
       <c r="D2772" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2773" spans="1:4" x14ac:dyDescent="0.25">
@@ -52183,7 +52180,7 @@
         <v>4294</v>
       </c>
       <c r="D2773" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2774" spans="1:4" x14ac:dyDescent="0.25">
@@ -52281,7 +52278,7 @@
         <v>2600</v>
       </c>
       <c r="D2780" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2781" spans="1:4" x14ac:dyDescent="0.25">
@@ -52939,7 +52936,7 @@
         <v>4306</v>
       </c>
       <c r="D2827" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2828" spans="1:4" x14ac:dyDescent="0.25">
@@ -52995,7 +52992,7 @@
         <v>1682</v>
       </c>
       <c r="D2831" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2832" spans="1:4" x14ac:dyDescent="0.25">
@@ -53009,7 +53006,7 @@
         <v>1682</v>
       </c>
       <c r="D2832" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2833" spans="1:4" x14ac:dyDescent="0.25">
@@ -53023,7 +53020,7 @@
         <v>4283</v>
       </c>
       <c r="D2833" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2834" spans="1:4" x14ac:dyDescent="0.25">
@@ -53037,7 +53034,7 @@
         <v>4294</v>
       </c>
       <c r="D2834" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2835" spans="1:4" x14ac:dyDescent="0.25">
@@ -53233,7 +53230,7 @@
         <v>4270</v>
       </c>
       <c r="D2848" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2849" spans="1:4" x14ac:dyDescent="0.25">
@@ -53247,7 +53244,7 @@
         <v>4270</v>
       </c>
       <c r="D2849" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2850" spans="1:4" x14ac:dyDescent="0.25">
@@ -53261,7 +53258,7 @@
         <v>4270</v>
       </c>
       <c r="D2850" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2851" spans="1:4" x14ac:dyDescent="0.25">
@@ -53667,7 +53664,7 @@
         <v>4306</v>
       </c>
       <c r="D2879" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2880" spans="1:4" x14ac:dyDescent="0.25">
@@ -53681,7 +53678,7 @@
         <v>286</v>
       </c>
       <c r="D2880" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="2881" spans="1:4" x14ac:dyDescent="0.25">
@@ -53947,7 +53944,7 @@
         <v>4294</v>
       </c>
       <c r="D2899" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2900" spans="1:4" x14ac:dyDescent="0.25">
@@ -53961,7 +53958,7 @@
         <v>4294</v>
       </c>
       <c r="D2900" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2901" spans="1:4" x14ac:dyDescent="0.25">
@@ -54003,7 +54000,7 @@
         <v>3225</v>
       </c>
       <c r="D2903" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2904" spans="1:4" x14ac:dyDescent="0.25">
@@ -54017,7 +54014,7 @@
         <v>3225</v>
       </c>
       <c r="D2904" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2905" spans="1:4" x14ac:dyDescent="0.25">
@@ -54059,7 +54056,7 @@
         <v>3230</v>
       </c>
       <c r="D2907" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2908" spans="1:4" x14ac:dyDescent="0.25">
@@ -54297,7 +54294,7 @@
         <v>4270</v>
       </c>
       <c r="D2924" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2925" spans="1:4" x14ac:dyDescent="0.25">
@@ -54311,7 +54308,7 @@
         <v>4294</v>
       </c>
       <c r="D2925" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2926" spans="1:4" x14ac:dyDescent="0.25">
@@ -54325,7 +54322,7 @@
         <v>4294</v>
       </c>
       <c r="D2926" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2927" spans="1:4" x14ac:dyDescent="0.25">
@@ -54409,7 +54406,7 @@
         <v>4294</v>
       </c>
       <c r="D2932" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2933" spans="1:4" x14ac:dyDescent="0.25">
@@ -54549,7 +54546,7 @@
         <v>286</v>
       </c>
       <c r="D2942" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="2943" spans="1:4" x14ac:dyDescent="0.25">
@@ -54633,7 +54630,7 @@
         <v>4294</v>
       </c>
       <c r="D2948" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2949" spans="1:4" x14ac:dyDescent="0.25">
@@ -54689,7 +54686,7 @@
         <v>4283</v>
       </c>
       <c r="D2952" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2953" spans="1:4" x14ac:dyDescent="0.25">
@@ -54703,7 +54700,7 @@
         <v>4283</v>
       </c>
       <c r="D2953" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2954" spans="1:4" x14ac:dyDescent="0.25">
@@ -54717,7 +54714,7 @@
         <v>1682</v>
       </c>
       <c r="D2954" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2955" spans="1:4" x14ac:dyDescent="0.25">
@@ -55039,7 +55036,7 @@
         <v>3302</v>
       </c>
       <c r="D2977" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2978" spans="1:4" x14ac:dyDescent="0.25">
@@ -55109,7 +55106,7 @@
         <v>3302</v>
       </c>
       <c r="D2982" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2983" spans="1:4" x14ac:dyDescent="0.25">
@@ -55193,7 +55190,7 @@
         <v>3230</v>
       </c>
       <c r="D2988" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="2989" spans="1:4" x14ac:dyDescent="0.25">
@@ -55655,7 +55652,7 @@
         <v>4294</v>
       </c>
       <c r="D3021" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3022" spans="1:4" x14ac:dyDescent="0.25">
@@ -55669,7 +55666,7 @@
         <v>450</v>
       </c>
       <c r="D3022" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3023" spans="1:4" x14ac:dyDescent="0.25">
@@ -55683,7 +55680,7 @@
         <v>4294</v>
       </c>
       <c r="D3023" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3024" spans="1:4" x14ac:dyDescent="0.25">
@@ -55697,7 +55694,7 @@
         <v>4270</v>
       </c>
       <c r="D3024" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3025" spans="1:4" x14ac:dyDescent="0.25">
@@ -55711,7 +55708,7 @@
         <v>4294</v>
       </c>
       <c r="D3025" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3026" spans="1:4" x14ac:dyDescent="0.25">
@@ -55725,7 +55722,7 @@
         <v>4294</v>
       </c>
       <c r="D3026" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3027" spans="1:4" x14ac:dyDescent="0.25">
@@ -55739,7 +55736,7 @@
         <v>4294</v>
       </c>
       <c r="D3027" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3028" spans="1:4" x14ac:dyDescent="0.25">
@@ -55753,7 +55750,7 @@
         <v>4294</v>
       </c>
       <c r="D3028" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3029" spans="1:4" x14ac:dyDescent="0.25">
@@ -55767,7 +55764,7 @@
         <v>3022</v>
       </c>
       <c r="D3029" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3030" spans="1:4" x14ac:dyDescent="0.25">
@@ -55879,7 +55876,7 @@
         <v>4294</v>
       </c>
       <c r="D3037" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3038" spans="1:4" x14ac:dyDescent="0.25">
@@ -55935,7 +55932,7 @@
         <v>4306</v>
       </c>
       <c r="D3041" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3042" spans="1:4" x14ac:dyDescent="0.25">
@@ -55949,7 +55946,7 @@
         <v>4306</v>
       </c>
       <c r="D3042" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3043" spans="1:4" x14ac:dyDescent="0.25">
@@ -55963,7 +55960,7 @@
         <v>4306</v>
       </c>
       <c r="D3043" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3044" spans="1:4" x14ac:dyDescent="0.25">
@@ -56033,7 +56030,7 @@
         <v>5</v>
       </c>
       <c r="D3048" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3049" spans="1:4" x14ac:dyDescent="0.25">
@@ -56341,7 +56338,7 @@
         <v>4283</v>
       </c>
       <c r="D3070" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3071" spans="1:4" x14ac:dyDescent="0.25">
@@ -56495,7 +56492,7 @@
         <v>4283</v>
       </c>
       <c r="D3081" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3082" spans="1:4" x14ac:dyDescent="0.25">
@@ -56663,7 +56660,7 @@
         <v>4294</v>
       </c>
       <c r="D3093" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3094" spans="1:4" x14ac:dyDescent="0.25">
@@ -56677,7 +56674,7 @@
         <v>4283</v>
       </c>
       <c r="D3094" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3095" spans="1:4" x14ac:dyDescent="0.25">
@@ -56691,7 +56688,7 @@
         <v>4283</v>
       </c>
       <c r="D3095" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3096" spans="1:4" x14ac:dyDescent="0.25">
@@ -57013,7 +57010,7 @@
         <v>3455</v>
       </c>
       <c r="D3118" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3119" spans="1:4" x14ac:dyDescent="0.25">
@@ -57125,7 +57122,7 @@
         <v>5</v>
       </c>
       <c r="D3126" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3127" spans="1:4" x14ac:dyDescent="0.25">
@@ -57181,7 +57178,7 @@
         <v>3455</v>
       </c>
       <c r="D3130" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3131" spans="1:4" x14ac:dyDescent="0.25">
@@ -57265,7 +57262,7 @@
         <v>214</v>
       </c>
       <c r="D3136" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3137" spans="1:4" x14ac:dyDescent="0.25">
@@ -57293,7 +57290,7 @@
         <v>286</v>
       </c>
       <c r="D3138" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3139" spans="1:4" x14ac:dyDescent="0.25">
@@ -57391,7 +57388,7 @@
         <v>3302</v>
       </c>
       <c r="D3145" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3146" spans="1:4" x14ac:dyDescent="0.25">
@@ -57405,7 +57402,7 @@
         <v>3302</v>
       </c>
       <c r="D3146" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3147" spans="1:4" x14ac:dyDescent="0.25">
@@ -57475,7 +57472,7 @@
         <v>2062</v>
       </c>
       <c r="D3151" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3152" spans="1:4" x14ac:dyDescent="0.25">
@@ -57489,7 +57486,7 @@
         <v>2062</v>
       </c>
       <c r="D3152" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3153" spans="1:4" x14ac:dyDescent="0.25">
@@ -57503,7 +57500,7 @@
         <v>2062</v>
       </c>
       <c r="D3153" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3154" spans="1:4" x14ac:dyDescent="0.25">
@@ -57769,7 +57766,7 @@
         <v>286</v>
       </c>
       <c r="D3172" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3173" spans="1:4" x14ac:dyDescent="0.25">
@@ -57783,7 +57780,7 @@
         <v>5</v>
       </c>
       <c r="D3173" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3174" spans="1:4" x14ac:dyDescent="0.25">
@@ -57923,7 +57920,7 @@
         <v>286</v>
       </c>
       <c r="D3183" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3184" spans="1:4" x14ac:dyDescent="0.25">
@@ -58007,7 +58004,7 @@
         <v>4294</v>
       </c>
       <c r="D3189" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3190" spans="1:4" x14ac:dyDescent="0.25">
@@ -58021,7 +58018,7 @@
         <v>4283</v>
       </c>
       <c r="D3190" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3191" spans="1:4" x14ac:dyDescent="0.25">
@@ -58035,7 +58032,7 @@
         <v>4283</v>
       </c>
       <c r="D3191" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3192" spans="1:4" x14ac:dyDescent="0.25">
@@ -58049,7 +58046,7 @@
         <v>3022</v>
       </c>
       <c r="D3192" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3193" spans="1:4" x14ac:dyDescent="0.25">
@@ -58063,7 +58060,7 @@
         <v>1682</v>
       </c>
       <c r="D3193" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3194" spans="1:4" x14ac:dyDescent="0.25">
@@ -58301,7 +58298,7 @@
         <v>643</v>
       </c>
       <c r="D3210" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3211" spans="1:4" x14ac:dyDescent="0.25">
@@ -58693,7 +58690,7 @@
         <v>2557</v>
       </c>
       <c r="D3238" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3239" spans="1:4" x14ac:dyDescent="0.25">
@@ -58763,7 +58760,7 @@
         <v>2215</v>
       </c>
       <c r="D3243" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3244" spans="1:4" x14ac:dyDescent="0.25">
@@ -59029,7 +59026,7 @@
         <v>4306</v>
       </c>
       <c r="D3262" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3263" spans="1:4" x14ac:dyDescent="0.25">
@@ -59393,7 +59390,7 @@
         <v>4294</v>
       </c>
       <c r="D3288" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3289" spans="1:4" x14ac:dyDescent="0.25">
@@ -59421,7 +59418,7 @@
         <v>450</v>
       </c>
       <c r="D3290" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3291" spans="1:4" x14ac:dyDescent="0.25">
@@ -59435,7 +59432,7 @@
         <v>4283</v>
       </c>
       <c r="D3291" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3292" spans="1:4" x14ac:dyDescent="0.25">
@@ -59449,7 +59446,7 @@
         <v>4283</v>
       </c>
       <c r="D3292" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3293" spans="1:4" x14ac:dyDescent="0.25">
@@ -59463,7 +59460,7 @@
         <v>4283</v>
       </c>
       <c r="D3293" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3294" spans="1:4" x14ac:dyDescent="0.25">
@@ -59477,7 +59474,7 @@
         <v>4283</v>
       </c>
       <c r="D3294" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3295" spans="1:4" x14ac:dyDescent="0.25">
@@ -59491,7 +59488,7 @@
         <v>4283</v>
       </c>
       <c r="D3295" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3296" spans="1:4" x14ac:dyDescent="0.25">
@@ -59505,7 +59502,7 @@
         <v>4283</v>
       </c>
       <c r="D3296" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3297" spans="1:4" x14ac:dyDescent="0.25">
@@ -59827,7 +59824,7 @@
         <v>3230</v>
       </c>
       <c r="D3319" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3320" spans="1:4" x14ac:dyDescent="0.25">
@@ -59981,7 +59978,7 @@
         <v>214</v>
       </c>
       <c r="D3330" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3331" spans="1:4" x14ac:dyDescent="0.25">
@@ -60023,7 +60020,7 @@
         <v>3022</v>
       </c>
       <c r="D3333" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3334" spans="1:4" x14ac:dyDescent="0.25">
@@ -60037,7 +60034,7 @@
         <v>3022</v>
       </c>
       <c r="D3334" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3335" spans="1:4" x14ac:dyDescent="0.25">
@@ -60261,7 +60258,7 @@
         <v>286</v>
       </c>
       <c r="D3350" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3351" spans="1:4" x14ac:dyDescent="0.25">
@@ -60625,7 +60622,7 @@
         <v>4294</v>
       </c>
       <c r="D3376" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3377" spans="1:4" x14ac:dyDescent="0.25">
@@ -60681,7 +60678,7 @@
         <v>3022</v>
       </c>
       <c r="D3380" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3381" spans="1:4" x14ac:dyDescent="0.25">
@@ -60695,7 +60692,7 @@
         <v>3022</v>
       </c>
       <c r="D3381" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3382" spans="1:4" x14ac:dyDescent="0.25">
@@ -61059,7 +61056,7 @@
         <v>3757</v>
       </c>
       <c r="D3407" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3408" spans="1:4" x14ac:dyDescent="0.25">
@@ -61073,7 +61070,7 @@
         <v>3757</v>
       </c>
       <c r="D3408" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3409" spans="1:4" x14ac:dyDescent="0.25">
@@ -61367,7 +61364,7 @@
         <v>3455</v>
       </c>
       <c r="D3429" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3430" spans="1:4" x14ac:dyDescent="0.25">
@@ -61409,7 +61406,7 @@
         <v>4294</v>
       </c>
       <c r="D3432" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3433" spans="1:4" x14ac:dyDescent="0.25">
@@ -61423,7 +61420,7 @@
         <v>4294</v>
       </c>
       <c r="D3433" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3434" spans="1:4" x14ac:dyDescent="0.25">
@@ -61437,7 +61434,7 @@
         <v>4294</v>
       </c>
       <c r="D3434" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3435" spans="1:4" x14ac:dyDescent="0.25">
@@ -61451,7 +61448,7 @@
         <v>2719</v>
       </c>
       <c r="D3435" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3436" spans="1:4" x14ac:dyDescent="0.25">
@@ -61465,7 +61462,7 @@
         <v>2719</v>
       </c>
       <c r="D3436" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3437" spans="1:4" x14ac:dyDescent="0.25">
@@ -61479,7 +61476,7 @@
         <v>1682</v>
       </c>
       <c r="D3437" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3438" spans="1:4" x14ac:dyDescent="0.25">
@@ -61493,7 +61490,7 @@
         <v>1682</v>
       </c>
       <c r="D3438" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3439" spans="1:4" x14ac:dyDescent="0.25">
@@ -61577,7 +61574,7 @@
         <v>3302</v>
       </c>
       <c r="D3444" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3445" spans="1:4" x14ac:dyDescent="0.25">
@@ -61829,7 +61826,7 @@
         <v>1849</v>
       </c>
       <c r="D3462" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3463" spans="1:4" x14ac:dyDescent="0.25">
@@ -61913,7 +61910,7 @@
         <v>4270</v>
       </c>
       <c r="D3468" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3469" spans="1:4" x14ac:dyDescent="0.25">
@@ -62207,7 +62204,7 @@
         <v>2600</v>
       </c>
       <c r="D3489" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3490" spans="1:4" x14ac:dyDescent="0.25">
@@ -62319,7 +62316,7 @@
         <v>4283</v>
       </c>
       <c r="D3497" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3498" spans="1:4" x14ac:dyDescent="0.25">
@@ -62515,7 +62512,7 @@
         <v>2557</v>
       </c>
       <c r="D3511" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3512" spans="1:4" x14ac:dyDescent="0.25">
@@ -62529,7 +62526,7 @@
         <v>2557</v>
       </c>
       <c r="D3512" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3513" spans="1:4" x14ac:dyDescent="0.25">
@@ -62585,7 +62582,7 @@
         <v>2557</v>
       </c>
       <c r="D3516" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3517" spans="1:4" x14ac:dyDescent="0.25">
@@ -62739,7 +62736,7 @@
         <v>4294</v>
       </c>
       <c r="D3527" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3528" spans="1:4" x14ac:dyDescent="0.25">
@@ -62753,7 +62750,7 @@
         <v>4294</v>
       </c>
       <c r="D3528" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3529" spans="1:4" x14ac:dyDescent="0.25">
@@ -62851,7 +62848,7 @@
         <v>4283</v>
       </c>
       <c r="D3535" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3536" spans="1:4" x14ac:dyDescent="0.25">
@@ -62865,7 +62862,7 @@
         <v>4294</v>
       </c>
       <c r="D3536" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3537" spans="1:4" x14ac:dyDescent="0.25">
@@ -62879,7 +62876,7 @@
         <v>4291</v>
       </c>
       <c r="D3537" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3538" spans="1:4" x14ac:dyDescent="0.25">
@@ -63103,7 +63100,7 @@
         <v>4283</v>
       </c>
       <c r="D3553" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3554" spans="1:4" x14ac:dyDescent="0.25">
@@ -63551,7 +63548,7 @@
         <v>4270</v>
       </c>
       <c r="D3585" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3586" spans="1:4" x14ac:dyDescent="0.25">
@@ -63565,7 +63562,7 @@
         <v>4270</v>
       </c>
       <c r="D3586" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3587" spans="1:4" x14ac:dyDescent="0.25">
@@ -64545,7 +64542,7 @@
         <v>643</v>
       </c>
       <c r="D3656" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3657" spans="1:4" x14ac:dyDescent="0.25">
@@ -64559,7 +64556,7 @@
         <v>3757</v>
       </c>
       <c r="D3657" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3658" spans="1:4" x14ac:dyDescent="0.25">
@@ -64573,7 +64570,7 @@
         <v>643</v>
       </c>
       <c r="D3658" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3659" spans="1:4" x14ac:dyDescent="0.25">
@@ -64587,7 +64584,7 @@
         <v>2600</v>
       </c>
       <c r="D3659" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3660" spans="1:4" x14ac:dyDescent="0.25">
@@ -64601,7 +64598,7 @@
         <v>2600</v>
       </c>
       <c r="D3660" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3661" spans="1:4" x14ac:dyDescent="0.25">
@@ -64643,7 +64640,7 @@
         <v>4283</v>
       </c>
       <c r="D3663" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3664" spans="1:4" x14ac:dyDescent="0.25">
@@ -64657,7 +64654,7 @@
         <v>4283</v>
       </c>
       <c r="D3664" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3665" spans="1:4" x14ac:dyDescent="0.25">
@@ -64671,7 +64668,7 @@
         <v>4283</v>
       </c>
       <c r="D3665" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3666" spans="1:4" x14ac:dyDescent="0.25">
@@ -64755,7 +64752,7 @@
         <v>4294</v>
       </c>
       <c r="D3671" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3672" spans="1:4" x14ac:dyDescent="0.25">
@@ -64769,7 +64766,7 @@
         <v>4294</v>
       </c>
       <c r="D3672" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3673" spans="1:4" x14ac:dyDescent="0.25">
@@ -65721,7 +65718,7 @@
         <v>450</v>
       </c>
       <c r="D3740" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3741" spans="1:4" x14ac:dyDescent="0.25">
@@ -65777,7 +65774,7 @@
         <v>4294</v>
       </c>
       <c r="D3744" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3745" spans="1:4" x14ac:dyDescent="0.25">
@@ -65791,7 +65788,7 @@
         <v>3022</v>
       </c>
       <c r="D3745" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3746" spans="1:4" x14ac:dyDescent="0.25">
@@ -65805,7 +65802,7 @@
         <v>4283</v>
       </c>
       <c r="D3746" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3747" spans="1:4" x14ac:dyDescent="0.25">
@@ -65819,7 +65816,7 @@
         <v>4294</v>
       </c>
       <c r="D3747" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3748" spans="1:4" x14ac:dyDescent="0.25">
@@ -65833,7 +65830,7 @@
         <v>4283</v>
       </c>
       <c r="D3748" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3749" spans="1:4" x14ac:dyDescent="0.25">
@@ -65847,7 +65844,7 @@
         <v>4294</v>
       </c>
       <c r="D3749" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3750" spans="1:4" x14ac:dyDescent="0.25">
@@ -65931,7 +65928,7 @@
         <v>450</v>
       </c>
       <c r="D3755" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3756" spans="1:4" x14ac:dyDescent="0.25">
@@ -66519,7 +66516,7 @@
         <v>214</v>
       </c>
       <c r="D3797" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3798" spans="1:4" x14ac:dyDescent="0.25">
@@ -66617,7 +66614,7 @@
         <v>4283</v>
       </c>
       <c r="D3804" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3805" spans="1:4" x14ac:dyDescent="0.25">
@@ -67023,7 +67020,7 @@
         <v>4294</v>
       </c>
       <c r="D3833" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3834" spans="1:4" x14ac:dyDescent="0.25">
@@ -67037,7 +67034,7 @@
         <v>4294</v>
       </c>
       <c r="D3834" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3835" spans="1:4" x14ac:dyDescent="0.25">
@@ -67051,7 +67048,7 @@
         <v>4294</v>
       </c>
       <c r="D3835" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3836" spans="1:4" x14ac:dyDescent="0.25">
@@ -67065,7 +67062,7 @@
         <v>4294</v>
       </c>
       <c r="D3836" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3837" spans="1:4" x14ac:dyDescent="0.25">
@@ -67079,7 +67076,7 @@
         <v>4294</v>
       </c>
       <c r="D3837" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3838" spans="1:4" x14ac:dyDescent="0.25">
@@ -67135,7 +67132,7 @@
         <v>4306</v>
       </c>
       <c r="D3841" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3842" spans="1:4" x14ac:dyDescent="0.25">
@@ -67555,7 +67552,7 @@
         <v>5</v>
       </c>
       <c r="D3871" s="2" t="s">
-        <v>4315</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="3872" spans="1:4" x14ac:dyDescent="0.25">
@@ -67597,7 +67594,7 @@
         <v>4283</v>
       </c>
       <c r="D3874" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3875" spans="1:4" x14ac:dyDescent="0.25">
@@ -67611,7 +67608,7 @@
         <v>4283</v>
       </c>
       <c r="D3875" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3876" spans="1:4" x14ac:dyDescent="0.25">
@@ -67667,7 +67664,7 @@
         <v>3230</v>
       </c>
       <c r="D3879" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3880" spans="1:4" x14ac:dyDescent="0.25">
@@ -67793,7 +67790,7 @@
         <v>4294</v>
       </c>
       <c r="D3888" s="2" t="s">
-        <v>4316</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="3889" spans="1:4" x14ac:dyDescent="0.25">
@@ -67924,7 +67921,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D3897">
-    <sortCondition ref="A1:A3897"/>
+    <sortCondition ref="A2644:A3897"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>